<commit_message>
Implemented the sell functionality, enabling users to process beverage sales and update inventory in real-time.
</commit_message>
<xml_diff>
--- a/sales.xlsx
+++ b/sales.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
@@ -706,42 +706,82 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>c40f6909-09f5-4ded-85c2-c5c153f7502b</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="1" t="inlineStr">
         <is>
           <t>OOREDOO</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="1" t="inlineStr">
         <is>
           <t>SIM Card</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="1" t="inlineStr">
         <is>
           <t>DIMA</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="1" t="inlineStr">
         <is>
           <t>1000</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G7" s="1" t="inlineStr">
         <is>
           <t>2024-09-10</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H7" s="1" t="inlineStr">
         <is>
           <t>22:01:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>95d64029-3b57-46ea-b0a6-8f8f87821cdc</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>xksksjd</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Soft Drinks</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>7UP</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2024-09-14</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>15:47:20</t>
         </is>
       </c>
     </row>

</xml_diff>